<commit_message>
run batch of camera postions
</commit_message>
<xml_diff>
--- a/in/2cam_impulse.xlsx
+++ b/in/2cam_impulse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -1263,7 +1263,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="1" sqref="B1 C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1895,7 +1895,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="1" sqref="B1 A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9008,10 +9008,10 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="1" sqref="B1 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9147,7 +9147,7 @@
         <v>123</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>8000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9155,7 +9155,7 @@
         <v>124</v>
       </c>
       <c r="B12" s="56" t="n">
-        <v>1100000000000</v>
+        <v>100000</v>
       </c>
       <c r="C12" s="56"/>
       <c r="D12" s="56"/>
@@ -9214,10 +9214,10 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C1" activeCellId="1" sqref="B1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9350,7 +9350,7 @@
         <v>123</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>8000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9358,7 +9358,7 @@
         <v>124</v>
       </c>
       <c r="C12" s="56" t="n">
-        <v>1100000000000</v>
+        <v>500000</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>

</xml_diff>

<commit_message>
titling, labeling, directory names
</commit_message>
<xml_diff>
--- a/in/2cam_impulse.xlsx
+++ b/in/2cam_impulse.xlsx
@@ -1263,7 +1263,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="1" sqref="B1 C38"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1895,7 +1895,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="1" sqref="B1 A35"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9011,7 +9011,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B11" activeCellId="1" sqref="B1 B11"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9217,7 +9217,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="1" sqref="B1 C1"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9264,6 +9264,7 @@
       <c r="A3" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="4" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
load L unless told otherwise
</commit_message>
<xml_diff>
--- a/in/2cam_impulse.xlsx
+++ b/in/2cam_impulse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -102,20 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Use this normally</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A38" authorId="0">
+    <comment ref="A35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="0">
+    <comment ref="A40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A61" authorId="0">
+    <comment ref="A58" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0">
+    <comment ref="A63" authorId="0">
       <text>
         <r>
           <rPr>
@@ -269,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="130">
   <si>
     <t xml:space="preserve">Sim</t>
   </si>
@@ -410,12 +397,6 @@
   </si>
   <si>
     <t xml:space="preserve">verfn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saveEll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loadEll</t>
   </si>
   <si>
     <t xml:space="preserve">RayAngleMapping</t>
@@ -677,7 +658,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -771,14 +752,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Sans"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
@@ -815,14 +788,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF3333"/>
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF3333"/>
       </patternFill>
     </fill>
   </fills>
@@ -951,7 +924,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1052,15 +1025,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1069,6 +1034,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,19 +1081,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1140,7 +1109,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1258,23 +1227,23 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.66836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.3724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,192 +1568,191 @@
       <c r="C34" s="5"/>
       <c r="F34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" s="26"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="22"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="A37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
       <c r="F37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="27" t="s">
-        <v>49</v>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B38" s="0"/>
-      <c r="C38" s="28" t="s">
-        <v>50</v>
-      </c>
+      <c r="C38" s="0"/>
       <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
       <c r="B39" s="0"/>
       <c r="C39" s="0"/>
       <c r="F39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="27" t="s">
         <v>51</v>
       </c>
       <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="F40" s="0"/>
+      <c r="C40" s="13"/>
+      <c r="F40" s="15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="28" t="s">
         <v>52</v>
       </c>
       <c r="B41" s="0"/>
       <c r="C41" s="0"/>
+      <c r="D41" s="29" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E41" s="30"/>
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4"/>
+      <c r="A42" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
-        <v>53</v>
+      <c r="A43" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="B43" s="0"/>
-      <c r="C43" s="13"/>
-      <c r="F43" s="15" t="n">
-        <v>1</v>
-      </c>
+      <c r="C43" s="0"/>
+      <c r="D43" s="31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="29" t="s">
-        <v>54</v>
+      <c r="A44" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
-      <c r="D44" s="30" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E44" s="31"/>
+      <c r="D44" s="31" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E44" s="32"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29" t="s">
-        <v>55</v>
+      <c r="A45" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="33"/>
+      <c r="D45" s="31" t="n">
+        <v>89</v>
+      </c>
+      <c r="E45" s="32"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="29" t="s">
-        <v>56</v>
+      <c r="A46" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="B46" s="0"/>
       <c r="C46" s="0"/>
-      <c r="D46" s="32" t="n">
-        <v>-3.8</v>
-      </c>
-      <c r="E46" s="33"/>
+      <c r="D46" s="33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E46" s="34"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
-        <v>57</v>
-      </c>
+      <c r="A47" s="4"/>
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
-      <c r="D47" s="32" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="E47" s="33"/>
-      <c r="F47" s="0"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B48" s="0"/>
       <c r="C48" s="0"/>
-      <c r="D48" s="32" t="n">
-        <v>89</v>
-      </c>
-      <c r="E48" s="33"/>
-      <c r="F48" s="0"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="29" t="s">
-        <v>59</v>
-      </c>
+      <c r="A49" s="4"/>
       <c r="B49" s="0"/>
       <c r="C49" s="0"/>
-      <c r="D49" s="34" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E49" s="35"/>
-      <c r="F49" s="0"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4"/>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="A50" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="7"/>
+      <c r="E50" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51" s="0"/>
       <c r="C51" s="0"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="15"/>
+      <c r="E51" s="5" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4"/>
+      <c r="A52" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B52" s="0"/>
       <c r="C52" s="0"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="7"/>
-      <c r="E53" s="0" t="s">
-        <v>62</v>
+      <c r="A53" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" s="0"/>
-      <c r="C54" s="0"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5" t="n">
-        <v>20</v>
-      </c>
+      <c r="A54" s="35"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
@@ -1792,8 +1760,6 @@
       </c>
       <c r="B55" s="0"/>
       <c r="C55" s="0"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
@@ -1801,34 +1767,30 @@
       </c>
       <c r="B56" s="0"/>
       <c r="C56" s="0"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5" t="n">
-        <v>800</v>
-      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="36"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
+      <c r="A57" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B59" s="0"/>
       <c r="C59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="A60" s="4"/>
       <c r="B60" s="0"/>
       <c r="C60" s="0"/>
     </row>
@@ -1838,39 +1800,20 @@
       </c>
       <c r="B61" s="0"/>
       <c r="C61" s="0"/>
+      <c r="E61" s="37"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="B62" s="0"/>
       <c r="C62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4"/>
-      <c r="B63" s="0"/>
-      <c r="C63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="A63" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="0"/>
-      <c r="C64" s="0"/>
-      <c r="E64" s="38"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0"/>
-      <c r="C65" s="0"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="5"/>
+      <c r="C63" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1900,18 +1843,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="21.9234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="39" width="23.3265306122449"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="39" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="38" width="22.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="38" width="23.6530612244898"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="38" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
-      <c r="B1" s="40" t="n">
+      <c r="B1" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="n">
+      <c r="C1" s="39" t="n">
         <v>1</v>
       </c>
       <c r="D1" s="0"/>
@@ -2165,7 +2108,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
@@ -2423,13 +2366,13 @@
       <c r="IQ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="41" t="n">
+      <c r="A3" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="41" t="n">
+      <c r="C3" s="40" t="n">
         <v>3.1436</v>
       </c>
       <c r="D3" s="0"/>
@@ -2682,13 +2625,13 @@
       <c r="IQ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="41" t="n">
+      <c r="A4" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="41" t="n">
+      <c r="C4" s="40" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="0"/>
@@ -2941,8 +2884,8 @@
       <c r="IQ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
-        <v>77</v>
+      <c r="A5" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>512</v>
@@ -3200,13 +3143,13 @@
       <c r="IQ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="41" t="n">
+      <c r="A6" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="40" t="n">
         <v>90</v>
       </c>
-      <c r="C6" s="41" t="n">
+      <c r="C6" s="40" t="n">
         <v>88.0172525718237</v>
       </c>
       <c r="D6" s="0"/>
@@ -3459,13 +3402,13 @@
       <c r="IQ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="41" t="n">
+      <c r="A7" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="40" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="41" t="n">
+      <c r="C7" s="40" t="n">
         <v>9</v>
       </c>
       <c r="D7" s="0"/>
@@ -3718,8 +3661,8 @@
       <c r="IQ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>80</v>
+      <c r="A8" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>1500</v>
@@ -3978,12 +3921,12 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="44" t="n">
+        <v>79</v>
+      </c>
+      <c r="B9" s="43" t="n">
         <v>250</v>
       </c>
-      <c r="C9" s="44" t="n">
+      <c r="C9" s="43" t="n">
         <v>250</v>
       </c>
       <c r="D9" s="0"/>
@@ -4237,10 +4180,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -4491,8 +4434,8 @@
       <c r="IQ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
-        <v>83</v>
+      <c r="A11" s="35" t="s">
+        <v>81</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -4747,9 +4690,9 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="45"/>
+        <v>82</v>
+      </c>
+      <c r="B12" s="44"/>
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
@@ -5002,7 +4945,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.02</v>
@@ -5260,13 +5203,13 @@
       <c r="IQ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="47" t="n">
+      <c r="A14" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="46" t="n">
         <v>-1</v>
       </c>
-      <c r="C14" s="47" t="n">
+      <c r="C14" s="46" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="0"/>
@@ -5519,11 +5462,11 @@
       <c r="IQ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="s">
-        <v>87</v>
+      <c r="A15" s="47" t="s">
+        <v>85</v>
       </c>
       <c r="B15" s="0"/>
-      <c r="C15" s="49"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
@@ -5774,11 +5717,11 @@
       <c r="IQ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="48" t="s">
-        <v>88</v>
+      <c r="A16" s="47" t="s">
+        <v>86</v>
       </c>
       <c r="B16" s="0"/>
-      <c r="C16" s="49"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
@@ -6029,11 +5972,11 @@
       <c r="IQ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
+      <c r="A17" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
@@ -6285,7 +6228,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -6541,7 +6484,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="0"/>
-      <c r="C19" s="53"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
@@ -6793,10 +6736,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="53"/>
+        <v>89</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
@@ -7048,10 +6991,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="53"/>
+        <v>90</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="0"/>
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
@@ -7303,7 +7246,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -7558,7 +7501,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -7813,7 +7756,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B9*0.9</f>
@@ -8327,7 +8270,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>15</v>
@@ -8586,7 +8529,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>2</v>
@@ -8850,7 +8793,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>512</v>
@@ -8861,7 +8804,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>512</v>
@@ -8872,7 +8815,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -8883,7 +8826,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -8894,7 +8837,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -8906,7 +8849,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>77.51</v>
@@ -8917,7 +8860,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>19.92</v>
@@ -8928,24 +8871,24 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8954,37 +8897,37 @@
       <c r="C39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="54" t="n">
+      <c r="A40" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C40" s="54" t="n">
+      <c r="C40" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="39" t="n">
+      <c r="A41" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="C41" s="39" t="n">
+      <c r="C41" s="38" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="39" t="n">
+      <c r="A42" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="C42" s="39" t="n">
+      <c r="C42" s="38" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9008,7 +8951,7 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -9016,8 +8959,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9038,25 +8981,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="55" t="n">
+      <c r="C2" s="54" t="n">
         <v>0.02</v>
       </c>
-      <c r="D2" s="55" t="n">
+      <c r="D2" s="54" t="n">
         <v>0.04</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1.75</v>
@@ -9070,21 +9013,21 @@
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>0.1</v>
@@ -9098,7 +9041,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>1</v>
@@ -9107,16 +9050,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -9125,16 +9068,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -9144,7 +9087,7 @@
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>5000</v>
@@ -9152,46 +9095,46 @@
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="56" t="n">
+        <v>122</v>
+      </c>
+      <c r="B12" s="55" t="n">
         <v>100000</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9222,8 +9165,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9244,25 +9187,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="55" t="n">
+      <c r="C2" s="54" t="n">
         <v>0.02</v>
       </c>
-      <c r="D2" s="55" t="n">
+      <c r="D2" s="54" t="n">
         <v>0.04</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="n">
@@ -9276,21 +9219,21 @@
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>0.1</v>
@@ -9303,7 +9246,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>1</v>
@@ -9311,16 +9254,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -9329,16 +9272,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -9348,7 +9291,7 @@
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>5000</v>
@@ -9356,45 +9299,45 @@
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="56" t="n">
+        <v>122</v>
+      </c>
+      <c r="C12" s="55" t="n">
         <v>500000</v>
       </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>